<commit_message>
Some bugs were detected
</commit_message>
<xml_diff>
--- a/testing/smoke.xlsx
+++ b/testing/smoke.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Documents\kr_aip\kr_aip\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9324AF-3E4B-43BE-B4ED-3BE554718A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C5DAD-4726-4945-B3E8-46D0A35C91F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F6CD83A6-9AE1-460D-A3E9-28D49D50CF90}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="241">
   <si>
     <t>status</t>
   </si>
@@ -705,9 +705,6 @@
     <t>Проверка пустого тела при редактировании</t>
   </si>
   <si>
-    <t>ВАЖНО ПРОДУМАТЬ ОГРАНИЧЕНИЯ НА ДЛИНЫ ПОЛЕЙ! ИНАЧЕ ПОЯВЛЯЮТСЯ ВЕСЬМА НЕОЧЕВИДНЫЕ БАГИ НА ФРОНТЕ</t>
-  </si>
-  <si>
     <t>Проверка значений реакций при редактировании</t>
   </si>
   <si>
@@ -715,6 +712,42 @@
   </si>
   <si>
     <t>Ввести в разные (и оба сразу) поля буквы и или символы</t>
+  </si>
+  <si>
+    <t>Подумать, стоит ли давать пользователю изменять пароль на тот же, что у него сейчас</t>
+  </si>
+  <si>
+    <t>Понятное отображение (подсветка красным) при создании поста без заголовка и тела</t>
+  </si>
+  <si>
+    <t>Не уверен, что после модерации стоит закрывать панель админки,</t>
+  </si>
+  <si>
+    <t>Не редактируется название поста: то есть можно ввести новое, но оно не отобразится, давайте отключим просто это</t>
+  </si>
+  <si>
+    <t>При добавлении длинной строки в тело поста, она некорректно отображается</t>
+  </si>
+  <si>
+    <t>При редактировании поста фокус идет на заднее окно, а не текущее, из-за этого не работает прокрутка мышью</t>
+  </si>
+  <si>
+    <t>Предложите что-то ещё, я бы писал через ё</t>
+  </si>
+  <si>
+    <t>Пропущен ь в добавьте</t>
+  </si>
+  <si>
+    <t>При задании пустого вопроса просто закрывается диалог, без уведомления об ошибке</t>
+  </si>
+  <si>
+    <t>При уходе корректного вопроса в админку, юзеру показать бы сообщение о модерации</t>
+  </si>
+  <si>
+    <t>При редактировании старого вопроса, я бы его не удалял (показывал бы старое тело) до модерации заново, это проблема не фронта, а общая</t>
+  </si>
+  <si>
+    <t>На анимации загрузки после обновления страницы первое подпрыгивание шарика быстрее</t>
   </si>
 </sst>
 </file>
@@ -770,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -781,14 +814,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,13 +832,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,6 +850,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1730829</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>123564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4016830</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>12172</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DFE2646-1152-0A0D-9560-1693C78A2B1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8294915" y="40836135"/>
+          <a:ext cx="5802086" cy="1739180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3951516</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>553169</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>28163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4F47829-1D3F-5519-6DA4-115BFAA913EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14031687" y="40788772"/>
+          <a:ext cx="4188996" cy="1987591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1837764</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>156308</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53788</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>112710</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97178CCB-6F0E-0978-0584-FD01BE0AF575}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8399929" y="41573249"/>
+          <a:ext cx="1739153" cy="1211461"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600636</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>24910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2079812</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>49529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12BE4C40-D61F-10FF-D092-91FD5CF9CE44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10685930" y="41621145"/>
+          <a:ext cx="1479176" cy="741796"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2043953</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>109709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3617716</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>993</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Рисунок 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45BCCF7A-57AF-8702-5FB5-AF70CE12FBB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12129247" y="41705944"/>
+          <a:ext cx="1573763" cy="608461"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1124,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566C57F2-AE52-49BB-91A0-D93A697A4BF7}">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:F236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A225" sqref="A225"/>
+    <sheetView tabSelected="1" topLeftCell="A225" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,16 +1410,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
@@ -1180,33 +1430,33 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1220,9 +1470,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" t="s">
         <v>14</v>
@@ -1230,9 +1480,9 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" t="s">
         <v>15</v>
@@ -1240,9 +1490,9 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" t="s">
         <v>16</v>
@@ -1250,13 +1500,13 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1270,9 +1520,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" t="s">
         <v>14</v>
@@ -1280,9 +1530,9 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" t="s">
         <v>15</v>
@@ -1290,9 +1540,9 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" t="s">
         <v>23</v>
@@ -1300,13 +1550,13 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>4</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1320,9 +1570,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" t="s">
         <v>14</v>
@@ -1330,9 +1580,9 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" t="s">
         <v>15</v>
@@ -1340,9 +1590,9 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" t="s">
         <v>26</v>
@@ -1350,13 +1600,13 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>5</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="A17" s="6">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1370,9 +1620,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" t="s">
         <v>14</v>
@@ -1380,9 +1630,9 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" t="s">
         <v>15</v>
@@ -1390,9 +1640,9 @@
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" t="s">
         <v>29</v>
@@ -1400,13 +1650,13 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>6</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -1420,9 +1670,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="7"/>
       <c r="E22" t="s">
         <v>14</v>
@@ -1430,9 +1680,9 @@
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="7"/>
       <c r="E23" t="s">
         <v>15</v>
@@ -1440,9 +1690,9 @@
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" t="s">
         <v>35</v>
@@ -1450,13 +1700,13 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+      <c r="A25" s="6">
         <v>7</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1470,9 +1720,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" t="s">
         <v>39</v>
@@ -1482,9 +1732,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" t="s">
         <v>40</v>
@@ -1494,9 +1744,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="7"/>
       <c r="E28" t="s">
         <v>41</v>
@@ -1526,13 +1776,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
+      <c r="A30" s="6">
         <v>9</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -1541,35 +1791,35 @@
       <c r="E30" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="8"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="7"/>
       <c r="E32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="8"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
+      <c r="A33" s="6">
         <v>10</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -1586,8 +1836,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="3" t="s">
@@ -1598,13 +1848,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
+      <c r="A35" s="6">
         <v>11</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="7" t="s">
@@ -1618,9 +1868,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" t="s">
         <v>63</v>
@@ -1630,140 +1880,140 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>12</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="11" t="s">
         <v>61</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="11"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
+      <c r="A39" s="8">
         <v>13</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="B39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="9"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="9"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
+      <c r="A43" s="8">
         <v>14</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="B43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="10"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="9"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="10"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="9"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="10"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F46" s="9"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
+      <c r="A47" s="6">
         <v>15</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -1775,25 +2025,25 @@
       <c r="E47" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
+      <c r="A49" s="6">
         <v>16</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -1805,25 +2055,25 @@
       <c r="E49" t="s">
         <v>81</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" t="s">
         <v>77</v>
       </c>
-      <c r="F50" s="8"/>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="8">
+      <c r="A51" s="6">
         <v>17</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -1835,25 +2085,25 @@
       <c r="E51" t="s">
         <v>83</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" t="s">
         <v>77</v>
       </c>
-      <c r="F52" s="8"/>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
+      <c r="A53" s="6">
         <v>18</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -1865,28 +2115,28 @@
       <c r="E53" t="s">
         <v>85</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" t="s">
         <v>86</v>
       </c>
-      <c r="F54" s="8"/>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
+      <c r="A55" s="6">
         <v>19</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="B55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>91</v>
       </c>
       <c r="D55" s="7" t="s">
@@ -1895,38 +2145,38 @@
       <c r="E55" t="s">
         <v>88</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
       <c r="D56" s="7"/>
       <c r="E56" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="8"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
       <c r="D57" s="7"/>
       <c r="E57" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="8"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="8">
+      <c r="A58" s="6">
         <v>20</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="8" t="s">
+      <c r="B58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D58" s="7" t="s">
@@ -1935,38 +2185,38 @@
       <c r="E58" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="7"/>
       <c r="E59" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="8"/>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
       <c r="D60" s="7"/>
       <c r="E60" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="8"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+      <c r="A61" s="6">
         <v>21</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="8" t="s">
+      <c r="B61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D61" s="7" t="s">
@@ -1975,38 +2225,38 @@
       <c r="E61" t="s">
         <v>92</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
       <c r="D62" s="7"/>
       <c r="E62" t="s">
         <v>88</v>
       </c>
-      <c r="F62" s="8"/>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
       <c r="D63" s="7"/>
       <c r="E63" t="s">
         <v>77</v>
       </c>
-      <c r="F63" s="8"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="8">
+      <c r="A64" s="6">
         <v>22</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="8" t="s">
+      <c r="B64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D64" s="7" t="s">
@@ -2015,50 +2265,50 @@
       <c r="E64" t="s">
         <v>93</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
       <c r="D65" s="7"/>
       <c r="E65" t="s">
         <v>89</v>
       </c>
-      <c r="F65" s="8"/>
+      <c r="F65" s="6"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
       <c r="D66" s="7"/>
       <c r="E66" t="s">
         <v>97</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F66" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
       <c r="D67" s="7"/>
       <c r="E67" t="s">
         <v>77</v>
       </c>
-      <c r="F67" s="8"/>
+      <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="8">
+      <c r="A68" s="6">
         <v>23</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="8" t="s">
+      <c r="B68" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>100</v>
       </c>
       <c r="D68" s="7" t="s">
@@ -2067,47 +2317,47 @@
       <c r="E68" t="s">
         <v>93</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F68" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
       <c r="D69" s="7"/>
       <c r="E69" t="s">
         <v>89</v>
       </c>
-      <c r="F69" s="8"/>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
       <c r="D70" s="7"/>
       <c r="E70" t="s">
         <v>101</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F70" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
       <c r="D71" s="7"/>
       <c r="E71" t="s">
         <v>77</v>
       </c>
-      <c r="F71" s="8"/>
+      <c r="F71" s="6"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="8">
+      <c r="A72" s="6">
         <v>24</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="7" t="s">
@@ -2119,50 +2369,50 @@
       <c r="E72" t="s">
         <v>93</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F72" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" t="s">
         <v>89</v>
       </c>
-      <c r="F73" s="6"/>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" t="s">
         <v>104</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" t="s">
         <v>77</v>
       </c>
-      <c r="F75" s="8"/>
+      <c r="F75" s="6"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="8">
+      <c r="A76" s="6">
         <v>25</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="8" t="s">
+      <c r="B76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D76" s="7" t="s">
@@ -2171,50 +2421,50 @@
       <c r="E76" t="s">
         <v>108</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F76" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
       <c r="D77" s="7"/>
       <c r="E77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="8"/>
+      <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8" t="s">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E78" t="s">
         <v>111</v>
       </c>
-      <c r="F78" s="8"/>
+      <c r="F78" s="6"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
       <c r="E79" t="s">
         <v>112</v>
       </c>
-      <c r="F79" s="8"/>
+      <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="8">
+      <c r="A80" s="6">
         <v>26</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="8" t="s">
+      <c r="B80" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D80" s="7" t="s">
@@ -2228,9 +2478,9 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="8"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
       <c r="D81" s="7"/>
       <c r="E81" t="s">
         <v>109</v>
@@ -2238,10 +2488,10 @@
       <c r="F81" s="7"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8" t="s">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E82" t="s">
@@ -2250,23 +2500,23 @@
       <c r="F82" s="7"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
       <c r="E83" t="s">
         <v>112</v>
       </c>
       <c r="F83" s="7"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="8">
+      <c r="A84" s="6">
         <v>27</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="8" t="s">
+      <c r="B84" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D84" s="7" t="s">
@@ -2275,151 +2525,151 @@
       <c r="E84" t="s">
         <v>108</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
       <c r="D85" s="7"/>
       <c r="E85" t="s">
         <v>109</v>
       </c>
-      <c r="F85" s="8"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E86" t="s">
         <v>114</v>
       </c>
-      <c r="F86" s="8"/>
+      <c r="F86" s="6"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
       <c r="E87" t="s">
         <v>112</v>
       </c>
-      <c r="F87" s="8"/>
+      <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="9">
+      <c r="A88" s="8">
         <v>28</v>
       </c>
-      <c r="B88" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="10" t="s">
+      <c r="B88" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="D88" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F88" s="9" t="s">
+      <c r="F88" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
       <c r="E89" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F89" s="9"/>
+      <c r="F89" s="8"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="9" t="s">
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F90" s="9"/>
+      <c r="F90" s="8"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="9"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="8"/>
       <c r="E91" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F91" s="9"/>
+      <c r="F91" s="8"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="9">
+      <c r="A92" s="8">
         <v>29</v>
       </c>
-      <c r="B92" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="10" t="s">
+      <c r="B92" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F92" s="9" t="s">
+      <c r="F92" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
       <c r="E93" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F93" s="9"/>
+      <c r="F93" s="8"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="9" t="s">
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F94" s="9"/>
+      <c r="F94" s="8"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="9"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="8"/>
       <c r="E95" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F95" s="9"/>
+      <c r="F95" s="8"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="8">
+      <c r="A96" s="6">
         <v>30</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="7" t="s">
@@ -2431,47 +2681,47 @@
       <c r="E96" t="s">
         <v>108</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="8"/>
-      <c r="B97" s="8"/>
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" t="s">
         <v>109</v>
       </c>
-      <c r="F97" s="8"/>
+      <c r="F97" s="6"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
       <c r="C98" s="7"/>
-      <c r="D98" s="8" t="s">
+      <c r="D98" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E98" t="s">
         <v>125</v>
       </c>
-      <c r="F98" s="8"/>
+      <c r="F98" s="6"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
       <c r="C99" s="7"/>
-      <c r="D99" s="8"/>
+      <c r="D99" s="6"/>
       <c r="E99" t="s">
         <v>112</v>
       </c>
-      <c r="F99" s="8"/>
+      <c r="F99" s="6"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="8">
+      <c r="A100" s="6">
         <v>31</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="7" t="s">
@@ -2483,50 +2733,50 @@
       <c r="E100" t="s">
         <v>108</v>
       </c>
-      <c r="F100" s="8" t="s">
+      <c r="F100" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" t="s">
         <v>109</v>
       </c>
-      <c r="F101" s="8"/>
+      <c r="F101" s="6"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="8"/>
-      <c r="B102" s="8"/>
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
       <c r="C102" s="7"/>
-      <c r="D102" s="8" t="s">
+      <c r="D102" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E102" t="s">
         <v>126</v>
       </c>
-      <c r="F102" s="8"/>
+      <c r="F102" s="6"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="8"/>
-      <c r="B103" s="8"/>
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
       <c r="C103" s="7"/>
-      <c r="D103" s="8"/>
+      <c r="D103" s="6"/>
       <c r="E103" t="s">
         <v>112</v>
       </c>
-      <c r="F103" s="8"/>
+      <c r="F103" s="6"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="8">
+      <c r="A104" s="6">
         <v>32</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="8" t="s">
+      <c r="B104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>127</v>
       </c>
       <c r="D104" s="7" t="s">
@@ -2535,52 +2785,52 @@
       <c r="E104" t="s">
         <v>108</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="F104" s="6" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
       <c r="D105" s="7"/>
       <c r="E105" t="s">
         <v>128</v>
       </c>
-      <c r="F105" s="8"/>
+      <c r="F105" s="6"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="8"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8" t="s">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F106" s="6" t="s">
+      <c r="F106" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
+      <c r="A107" s="6"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
       <c r="E107" t="s">
         <v>130</v>
       </c>
-      <c r="F107" s="6"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="8">
+      <c r="A108" s="6">
         <v>33</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="8" t="s">
+      <c r="B108" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D108" s="7" t="s">
@@ -2589,489 +2839,489 @@
       <c r="E108" t="s">
         <v>154</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F108" s="6" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
       <c r="D109" s="7"/>
       <c r="E109" t="s">
         <v>89</v>
       </c>
-      <c r="F109" s="8"/>
+      <c r="F109" s="6"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
       <c r="D110" s="7"/>
       <c r="E110" t="s">
         <v>156</v>
       </c>
-      <c r="F110" s="8" t="s">
+      <c r="F110" s="6" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
       <c r="D111" s="7"/>
       <c r="E111" t="s">
         <v>77</v>
       </c>
-      <c r="F111" s="8"/>
+      <c r="F111" s="6"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="8">
+      <c r="A112" s="6">
         <v>34</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="8" t="s">
+      <c r="B112" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D112" s="8" t="s">
+      <c r="D112" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E112" t="s">
         <v>135</v>
       </c>
-      <c r="F112" s="8" t="s">
+      <c r="F112" s="6" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
+      <c r="A113" s="6"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
       <c r="E113" t="s">
         <v>136</v>
       </c>
-      <c r="F113" s="8"/>
+      <c r="F113" s="6"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8" t="s">
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6" t="s">
         <v>134</v>
       </c>
       <c r="E114" t="s">
         <v>137</v>
       </c>
-      <c r="F114" s="8" t="s">
+      <c r="F114" s="6" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
       <c r="E115" t="s">
         <v>138</v>
       </c>
-      <c r="F115" s="8"/>
+      <c r="F115" s="6"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
       <c r="E116" t="s">
         <v>139</v>
       </c>
-      <c r="F116" s="8"/>
+      <c r="F116" s="6"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="8">
+      <c r="A117" s="6">
         <v>35</v>
       </c>
-      <c r="B117" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="8" t="s">
+      <c r="B117" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="D117" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E117" t="s">
         <v>135</v>
       </c>
-      <c r="F117" s="8" t="s">
+      <c r="F117" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
       <c r="E118" t="s">
         <v>136</v>
       </c>
-      <c r="F118" s="8"/>
+      <c r="F118" s="6"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8" t="s">
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6" t="s">
         <v>134</v>
       </c>
       <c r="E119" t="s">
         <v>137</v>
       </c>
-      <c r="F119" s="8"/>
+      <c r="F119" s="6"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
       <c r="E120" t="s">
         <v>143</v>
       </c>
-      <c r="F120" s="8"/>
+      <c r="F120" s="6"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="8"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
       <c r="E121" t="s">
         <v>139</v>
       </c>
-      <c r="F121" s="8"/>
+      <c r="F121" s="6"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="8">
+      <c r="A122" s="6">
         <v>36</v>
       </c>
-      <c r="B122" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="8" t="s">
+      <c r="B122" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D122" s="8" t="s">
+      <c r="D122" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E122" t="s">
         <v>135</v>
       </c>
-      <c r="F122" s="8" t="s">
+      <c r="F122" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
+      <c r="A123" s="6"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
       <c r="E123" t="s">
         <v>136</v>
       </c>
-      <c r="F123" s="8"/>
+      <c r="F123" s="6"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="8"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8" t="s">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6" t="s">
         <v>134</v>
       </c>
       <c r="E124" t="s">
         <v>146</v>
       </c>
-      <c r="F124" s="8"/>
+      <c r="F124" s="6"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="8"/>
-      <c r="B125" s="8"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
+      <c r="A125" s="6"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
       <c r="E125" t="s">
         <v>138</v>
       </c>
-      <c r="F125" s="8"/>
+      <c r="F125" s="6"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="8"/>
-      <c r="B126" s="8"/>
-      <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
       <c r="E126" t="s">
         <v>139</v>
       </c>
-      <c r="F126" s="8"/>
+      <c r="F126" s="6"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="11">
+      <c r="A127" s="10">
         <v>37</v>
       </c>
-      <c r="B127" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C127" s="12" t="s">
+      <c r="B127" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D127" s="11" t="s">
+      <c r="D127" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F127" s="11" t="s">
+      <c r="F127" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="12"/>
-      <c r="D128" s="11"/>
+      <c r="A128" s="10"/>
+      <c r="B128" s="10"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="10"/>
       <c r="E128" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F128" s="11"/>
+      <c r="F128" s="10"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="11"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="11" t="s">
+      <c r="A129" s="10"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="10" t="s">
         <v>134</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F129" s="11"/>
+      <c r="F129" s="10"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="11"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="12"/>
-      <c r="D130" s="11"/>
+      <c r="A130" s="10"/>
+      <c r="B130" s="10"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="10"/>
       <c r="E130" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F130" s="11"/>
+      <c r="F130" s="10"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="11"/>
-      <c r="B131" s="11"/>
-      <c r="C131" s="12"/>
-      <c r="D131" s="11"/>
+      <c r="A131" s="10"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="10"/>
       <c r="E131" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F131" s="11"/>
+      <c r="F131" s="10"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="11">
+      <c r="A132" s="10">
         <v>38</v>
       </c>
-      <c r="B132" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="B132" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D132" s="11" t="s">
+      <c r="D132" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F132" s="11" t="s">
+      <c r="F132" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="11"/>
-      <c r="B133" s="11"/>
-      <c r="C133" s="12"/>
-      <c r="D133" s="11"/>
+      <c r="A133" s="10"/>
+      <c r="B133" s="10"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="10"/>
       <c r="E133" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F133" s="11"/>
+      <c r="F133" s="10"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="11"/>
-      <c r="B134" s="11"/>
-      <c r="C134" s="12"/>
-      <c r="D134" s="11" t="s">
+      <c r="A134" s="10"/>
+      <c r="B134" s="10"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="10" t="s">
         <v>134</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F134" s="11"/>
+      <c r="F134" s="10"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11"/>
-      <c r="C135" s="12"/>
-      <c r="D135" s="11"/>
+      <c r="A135" s="10"/>
+      <c r="B135" s="10"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="10"/>
       <c r="E135" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F135" s="11"/>
+      <c r="F135" s="10"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="11"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="12"/>
-      <c r="D136" s="11"/>
+      <c r="A136" s="10"/>
+      <c r="B136" s="10"/>
+      <c r="C136" s="11"/>
+      <c r="D136" s="10"/>
       <c r="E136" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F136" s="11"/>
+      <c r="F136" s="10"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" s="11">
+      <c r="A137" s="10">
         <v>39</v>
       </c>
-      <c r="B137" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C137" s="12" t="s">
+      <c r="B137" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D137" s="11" t="s">
+      <c r="D137" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F137" s="11" t="s">
+      <c r="F137" s="10" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="12"/>
-      <c r="D138" s="11"/>
+      <c r="A138" s="10"/>
+      <c r="B138" s="10"/>
+      <c r="C138" s="11"/>
+      <c r="D138" s="10"/>
       <c r="E138" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F138" s="11"/>
+      <c r="F138" s="10"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" s="11"/>
-      <c r="B139" s="11"/>
-      <c r="C139" s="12"/>
-      <c r="D139" s="11" t="s">
+      <c r="A139" s="10"/>
+      <c r="B139" s="10"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="10" t="s">
         <v>134</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F139" s="11"/>
+      <c r="F139" s="10"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="12"/>
-      <c r="D140" s="11"/>
+      <c r="A140" s="10"/>
+      <c r="B140" s="10"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="10"/>
       <c r="E140" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F140" s="11"/>
+      <c r="F140" s="10"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" s="11"/>
-      <c r="B141" s="11"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="11"/>
+      <c r="A141" s="10"/>
+      <c r="B141" s="10"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="10"/>
       <c r="E141" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F141" s="11"/>
+      <c r="F141" s="10"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A142" s="9">
+      <c r="A142" s="8">
         <v>40</v>
       </c>
-      <c r="B142" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C142" s="9" t="s">
+      <c r="B142" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D142" s="9" t="s">
+      <c r="D142" s="8" t="s">
         <v>180</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F142" s="10" t="s">
+      <c r="F142" s="9" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="9"/>
-      <c r="D143" s="9"/>
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
       <c r="E143" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F143" s="10"/>
+      <c r="F143" s="9"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" s="9"/>
-      <c r="B144" s="9"/>
-      <c r="C144" s="9"/>
-      <c r="D144" s="10" t="s">
+      <c r="A144" s="8"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="9" t="s">
         <v>181</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="F144" s="10"/>
+      <c r="F144" s="9"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A145" s="9"/>
-      <c r="B145" s="9"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="10"/>
+      <c r="A145" s="8"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+      <c r="D145" s="9"/>
       <c r="E145" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F145" s="10"/>
+      <c r="F145" s="9"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" s="9"/>
-      <c r="B146" s="9"/>
-      <c r="C146" s="9"/>
-      <c r="D146" s="10"/>
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="9"/>
       <c r="E146" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="F146" s="10"/>
+      <c r="F146" s="9"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" s="8">
+      <c r="A147" s="6">
         <v>41</v>
       </c>
-      <c r="B147" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" s="8" t="s">
+      <c r="B147" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="D147" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E147" t="s">
@@ -3082,19 +3332,19 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A148" s="8"/>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
       <c r="E148" t="s">
         <v>160</v>
       </c>
       <c r="F148" s="7"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
       <c r="D149" s="7" t="s">
         <v>181</v>
       </c>
@@ -3104,9 +3354,9 @@
       <c r="F149" s="7"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" s="8"/>
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
       <c r="D150" s="7"/>
       <c r="E150" t="s">
         <v>162</v>
@@ -3114,9 +3364,9 @@
       <c r="F150" s="7"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" s="8"/>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
       <c r="D151" s="7"/>
       <c r="E151" t="s">
         <v>163</v>
@@ -3124,16 +3374,16 @@
       <c r="F151" s="7"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="8">
+      <c r="A152" s="6">
         <v>42</v>
       </c>
-      <c r="B152" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C152" s="8" t="s">
+      <c r="B152" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D152" s="8" t="s">
+      <c r="D152" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E152" t="s">
@@ -3144,19 +3394,19 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="8"/>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
       <c r="E153" t="s">
         <v>160</v>
       </c>
       <c r="F153" s="7"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
       <c r="D154" s="7" t="s">
         <v>181</v>
       </c>
@@ -3166,9 +3416,9 @@
       <c r="F154" s="7"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
       <c r="D155" s="7"/>
       <c r="E155" t="s">
         <v>162</v>
@@ -3176,9 +3426,9 @@
       <c r="F155" s="7"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
       <c r="D156" s="7"/>
       <c r="E156" t="s">
         <v>163</v>
@@ -3186,16 +3436,16 @@
       <c r="F156" s="7"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="8">
+      <c r="A157" s="6">
         <v>43</v>
       </c>
-      <c r="B157" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C157" s="8" t="s">
+      <c r="B157" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D157" s="8" t="s">
+      <c r="D157" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E157" t="s">
@@ -3206,19 +3456,19 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="8"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
       <c r="E158" t="s">
         <v>160</v>
       </c>
       <c r="F158" s="7"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="8"/>
-      <c r="B159" s="8"/>
-      <c r="C159" s="8"/>
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
       <c r="D159" s="7" t="s">
         <v>181</v>
       </c>
@@ -3228,9 +3478,9 @@
       <c r="F159" s="7"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="8"/>
-      <c r="B160" s="8"/>
-      <c r="C160" s="8"/>
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
       <c r="D160" s="7"/>
       <c r="E160" t="s">
         <v>173</v>
@@ -3238,9 +3488,9 @@
       <c r="F160" s="7"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A161" s="8"/>
-      <c r="B161" s="8"/>
-      <c r="C161" s="8"/>
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
       <c r="D161" s="7"/>
       <c r="E161" t="s">
         <v>163</v>
@@ -3248,16 +3498,16 @@
       <c r="F161" s="7"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A162" s="8">
+      <c r="A162" s="6">
         <v>44</v>
       </c>
-      <c r="B162" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C162" s="8" t="s">
+      <c r="B162" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D162" s="8" t="s">
+      <c r="D162" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E162" t="s">
@@ -3268,19 +3518,19 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="8"/>
-      <c r="B163" s="8"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
       <c r="E163" t="s">
         <v>160</v>
       </c>
       <c r="F163" s="7"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="8"/>
-      <c r="B164" s="8"/>
-      <c r="C164" s="8"/>
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
       <c r="D164" s="7" t="s">
         <v>181</v>
       </c>
@@ -3290,9 +3540,9 @@
       <c r="F164" s="7"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="8"/>
-      <c r="B165" s="8"/>
-      <c r="C165" s="8"/>
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
       <c r="D165" s="7"/>
       <c r="E165" t="s">
         <v>177</v>
@@ -3300,9 +3550,9 @@
       <c r="F165" s="7"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A166" s="8"/>
-      <c r="B166" s="8"/>
-      <c r="C166" s="8"/>
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
       <c r="D166" s="7"/>
       <c r="E166" t="s">
         <v>163</v>
@@ -3310,13 +3560,13 @@
       <c r="F166" s="7"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A167" s="8">
+      <c r="A167" s="6">
         <v>45</v>
       </c>
-      <c r="B167" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C167" s="8" t="s">
+      <c r="B167" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C167" s="6" t="s">
         <v>179</v>
       </c>
       <c r="D167" t="s">
@@ -3325,40 +3575,40 @@
       <c r="E167" t="s">
         <v>159</v>
       </c>
-      <c r="F167" s="6" t="s">
+      <c r="F167" s="12" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A168" s="8"/>
-      <c r="B168" s="8"/>
-      <c r="C168" s="8"/>
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
       <c r="D168" s="7" t="s">
         <v>182</v>
       </c>
       <c r="E168" t="s">
         <v>183</v>
       </c>
-      <c r="F168" s="6"/>
+      <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A169" s="8"/>
-      <c r="B169" s="8"/>
-      <c r="C169" s="8"/>
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
       <c r="D169" s="7"/>
       <c r="E169" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F169" s="6"/>
+      <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A170" s="8">
+      <c r="A170" s="6">
         <v>46</v>
       </c>
-      <c r="B170" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C170" s="8" t="s">
+      <c r="B170" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170" s="6" t="s">
         <v>186</v>
       </c>
       <c r="D170" t="s">
@@ -3372,9 +3622,9 @@
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A171" s="8"/>
-      <c r="B171" s="8"/>
-      <c r="C171" s="8"/>
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
       <c r="D171" t="s">
         <v>187</v>
       </c>
@@ -3386,10 +3636,10 @@
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A172" s="8"/>
-      <c r="B172" s="8"/>
-      <c r="C172" s="8"/>
-      <c r="D172" s="8" t="s">
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E172" t="s">
@@ -3400,10 +3650,10 @@
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A173" s="8"/>
-      <c r="B173" s="8"/>
-      <c r="C173" s="8"/>
-      <c r="D173" s="8"/>
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
       <c r="E173" t="s">
         <v>191</v>
       </c>
@@ -3412,10 +3662,10 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="8">
+      <c r="A174" s="6">
         <v>47</v>
       </c>
-      <c r="B174" s="8" t="s">
+      <c r="B174" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C174" s="7" t="s">
@@ -3427,13 +3677,13 @@
       <c r="E174" t="s">
         <v>188</v>
       </c>
-      <c r="F174" s="8" t="s">
+      <c r="F174" s="6" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="8"/>
-      <c r="B175" s="8"/>
+      <c r="A175" s="6"/>
+      <c r="B175" s="6"/>
       <c r="C175" s="7"/>
       <c r="D175" t="s">
         <v>187</v>
@@ -3441,37 +3691,37 @@
       <c r="E175" t="s">
         <v>189</v>
       </c>
-      <c r="F175" s="8"/>
+      <c r="F175" s="6"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="8"/>
-      <c r="B176" s="8"/>
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
       <c r="C176" s="7"/>
-      <c r="D176" s="8" t="s">
+      <c r="D176" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E176" t="s">
         <v>197</v>
       </c>
-      <c r="F176" s="8" t="s">
+      <c r="F176" s="6" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="8"/>
-      <c r="B177" s="8"/>
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
       <c r="C177" s="7"/>
-      <c r="D177" s="8"/>
+      <c r="D177" s="6"/>
       <c r="E177" t="s">
         <v>191</v>
       </c>
-      <c r="F177" s="8"/>
+      <c r="F177" s="6"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="8">
+      <c r="A178" s="6">
         <v>48</v>
       </c>
-      <c r="B178" s="8" t="s">
+      <c r="B178" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C178" s="7" t="s">
@@ -3483,13 +3733,13 @@
       <c r="E178" t="s">
         <v>188</v>
       </c>
-      <c r="F178" s="8" t="s">
+      <c r="F178" s="6" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A179" s="8"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
       <c r="C179" s="7"/>
       <c r="D179" t="s">
         <v>187</v>
@@ -3497,37 +3747,37 @@
       <c r="E179" t="s">
         <v>201</v>
       </c>
-      <c r="F179" s="8"/>
+      <c r="F179" s="6"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="8"/>
-      <c r="B180" s="8"/>
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
       <c r="C180" s="7"/>
-      <c r="D180" s="8" t="s">
+      <c r="D180" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E180" t="s">
         <v>190</v>
       </c>
-      <c r="F180" s="8" t="s">
+      <c r="F180" s="6" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="8"/>
-      <c r="B181" s="8"/>
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
       <c r="C181" s="7"/>
-      <c r="D181" s="8"/>
+      <c r="D181" s="6"/>
       <c r="E181" t="s">
         <v>191</v>
       </c>
-      <c r="F181" s="8"/>
+      <c r="F181" s="6"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="8">
+      <c r="A182" s="6">
         <v>49</v>
       </c>
-      <c r="B182" s="8" t="s">
+      <c r="B182" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C182" s="7" t="s">
@@ -3539,13 +3789,13 @@
       <c r="E182" t="s">
         <v>188</v>
       </c>
-      <c r="F182" s="8" t="s">
+      <c r="F182" s="6" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="8"/>
-      <c r="B183" s="8"/>
+      <c r="A183" s="6"/>
+      <c r="B183" s="6"/>
       <c r="C183" s="7"/>
       <c r="D183" t="s">
         <v>187</v>
@@ -3553,40 +3803,40 @@
       <c r="E183" t="s">
         <v>203</v>
       </c>
-      <c r="F183" s="8"/>
+      <c r="F183" s="6"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="8"/>
-      <c r="B184" s="8"/>
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
       <c r="C184" s="7"/>
-      <c r="D184" s="8" t="s">
+      <c r="D184" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E184" t="s">
         <v>190</v>
       </c>
-      <c r="F184" s="8" t="s">
+      <c r="F184" s="6" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A185" s="8"/>
-      <c r="B185" s="8"/>
+      <c r="A185" s="6"/>
+      <c r="B185" s="6"/>
       <c r="C185" s="7"/>
-      <c r="D185" s="8"/>
+      <c r="D185" s="6"/>
       <c r="E185" t="s">
         <v>191</v>
       </c>
-      <c r="F185" s="8"/>
+      <c r="F185" s="6"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="9">
+      <c r="A186" s="8">
         <v>50</v>
       </c>
-      <c r="B186" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C186" s="9" t="s">
+      <c r="B186" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186" s="8" t="s">
         <v>204</v>
       </c>
       <c r="D186" s="5" t="s">
@@ -3595,606 +3845,591 @@
       <c r="E186" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F186" s="9" t="s">
+      <c r="F186" s="8" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="9"/>
-      <c r="B187" s="9"/>
-      <c r="C187" s="9"/>
+      <c r="A187" s="8"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="8"/>
       <c r="D187" s="5" t="s">
         <v>187</v>
       </c>
       <c r="E187" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F187" s="9"/>
+      <c r="F187" s="8"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9"/>
-      <c r="C188" s="9"/>
-      <c r="D188" s="9" t="s">
+      <c r="A188" s="8"/>
+      <c r="B188" s="8"/>
+      <c r="C188" s="8"/>
+      <c r="D188" s="8" t="s">
         <v>180</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="F188" s="9" t="s">
+      <c r="F188" s="8" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" s="9"/>
-      <c r="B189" s="9"/>
-      <c r="C189" s="9"/>
-      <c r="D189" s="9"/>
+      <c r="A189" s="8"/>
+      <c r="B189" s="8"/>
+      <c r="C189" s="8"/>
+      <c r="D189" s="8"/>
       <c r="E189" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="F189" s="9"/>
+      <c r="F189" s="8"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" s="8">
+      <c r="A190" s="6">
         <v>51</v>
       </c>
-      <c r="B190" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C190" s="8" t="s">
+      <c r="B190" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D190" s="8" t="s">
+      <c r="D190" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E190" s="13" t="s">
+      <c r="E190" t="s">
         <v>209</v>
       </c>
-      <c r="F190" s="15" t="s">
+      <c r="F190" s="6" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A191" s="8"/>
-      <c r="B191" s="8"/>
-      <c r="C191" s="8"/>
-      <c r="D191" s="8"/>
-      <c r="E191" s="14" t="s">
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+      <c r="E191" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F191" s="15"/>
+      <c r="F191" s="6"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A192" s="8">
+      <c r="A192" s="6">
         <v>52</v>
       </c>
-      <c r="B192" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C192" s="8" t="s">
+      <c r="B192" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C192" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D192" s="8" t="s">
+      <c r="D192" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E192" s="13" t="s">
+      <c r="E192" t="s">
         <v>213</v>
       </c>
-      <c r="F192" s="15" t="s">
+      <c r="F192" s="6" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" s="8"/>
-      <c r="B193" s="8"/>
-      <c r="C193" s="8"/>
-      <c r="D193" s="8"/>
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
       <c r="E193" t="s">
         <v>214</v>
       </c>
-      <c r="F193" s="15"/>
+      <c r="F193" s="6"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="8"/>
-      <c r="B194" s="8"/>
-      <c r="C194" s="8"/>
-      <c r="D194" s="8"/>
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
       <c r="E194" t="s">
         <v>215</v>
       </c>
-      <c r="F194" s="15"/>
+      <c r="F194" s="6"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" s="8"/>
-      <c r="B195" s="8"/>
-      <c r="C195" s="8"/>
-      <c r="D195" s="8"/>
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
       <c r="E195" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F195" s="15"/>
+      <c r="F195" s="6"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A196" s="8"/>
-      <c r="B196" s="8"/>
-      <c r="C196" s="8"/>
-      <c r="D196" s="8"/>
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
       <c r="E196" t="s">
         <v>217</v>
       </c>
-      <c r="F196" s="15"/>
+      <c r="F196" s="6"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A197" s="8"/>
-      <c r="B197" s="8"/>
-      <c r="C197" s="8"/>
-      <c r="D197" s="8"/>
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
       <c r="E197" t="s">
         <v>163</v>
       </c>
-      <c r="F197" s="15"/>
+      <c r="F197" s="6"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" s="8">
+      <c r="A198" s="6">
         <v>53</v>
       </c>
-      <c r="B198" s="8" t="s">
+      <c r="B198" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C198" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D198" s="8" t="s">
+      <c r="D198" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E198" s="13" t="s">
+      <c r="E198" t="s">
         <v>213</v>
       </c>
-      <c r="F198" s="15" t="s">
+      <c r="F198" s="6" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" s="8"/>
-      <c r="B199" s="8"/>
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
       <c r="C199" s="7"/>
-      <c r="D199" s="8"/>
+      <c r="D199" s="6"/>
       <c r="E199" t="s">
         <v>214</v>
       </c>
-      <c r="F199" s="15"/>
+      <c r="F199" s="6"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A200" s="8"/>
-      <c r="B200" s="8"/>
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
       <c r="C200" s="7"/>
-      <c r="D200" s="8"/>
+      <c r="D200" s="6"/>
       <c r="E200" t="s">
         <v>215</v>
       </c>
-      <c r="F200" s="15"/>
+      <c r="F200" s="6"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" s="8"/>
-      <c r="B201" s="8"/>
+      <c r="A201" s="6"/>
+      <c r="B201" s="6"/>
       <c r="C201" s="7"/>
-      <c r="D201" s="8"/>
+      <c r="D201" s="6"/>
       <c r="E201" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F201" s="15"/>
+      <c r="F201" s="6"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="8"/>
-      <c r="B202" s="8"/>
+      <c r="A202" s="6"/>
+      <c r="B202" s="6"/>
       <c r="C202" s="7"/>
-      <c r="D202" s="8"/>
+      <c r="D202" s="6"/>
       <c r="E202" t="s">
         <v>220</v>
       </c>
-      <c r="F202" s="15"/>
+      <c r="F202" s="6"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" s="8"/>
-      <c r="B203" s="8"/>
+      <c r="A203" s="6"/>
+      <c r="B203" s="6"/>
       <c r="C203" s="7"/>
-      <c r="D203" s="8"/>
+      <c r="D203" s="6"/>
       <c r="E203" t="s">
         <v>163</v>
       </c>
-      <c r="F203" s="15"/>
+      <c r="F203" s="6"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" s="9">
+      <c r="A204" s="8">
         <v>54</v>
       </c>
-      <c r="B204" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C204" s="10" t="s">
+      <c r="B204" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C204" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="D204" s="9" t="s">
+      <c r="D204" s="8" t="s">
         <v>207</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F204" s="10" t="s">
+      <c r="F204" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" s="9"/>
-      <c r="B205" s="9"/>
-      <c r="C205" s="10"/>
-      <c r="D205" s="9"/>
+      <c r="A205" s="8"/>
+      <c r="B205" s="8"/>
+      <c r="C205" s="9"/>
+      <c r="D205" s="8"/>
       <c r="E205" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F205" s="10"/>
+      <c r="F205" s="9"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="9"/>
-      <c r="B206" s="9"/>
-      <c r="C206" s="10"/>
-      <c r="D206" s="9"/>
+      <c r="A206" s="8"/>
+      <c r="B206" s="8"/>
+      <c r="C206" s="9"/>
+      <c r="D206" s="8"/>
       <c r="E206" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F206" s="10"/>
+      <c r="F206" s="9"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A207" s="9"/>
-      <c r="B207" s="9"/>
-      <c r="C207" s="10"/>
-      <c r="D207" s="9"/>
+      <c r="A207" s="8"/>
+      <c r="B207" s="8"/>
+      <c r="C207" s="9"/>
+      <c r="D207" s="8"/>
       <c r="E207" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F207" s="10"/>
+      <c r="F207" s="9"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A208" s="9"/>
-      <c r="B208" s="9"/>
-      <c r="C208" s="10"/>
-      <c r="D208" s="9"/>
+      <c r="A208" s="8"/>
+      <c r="B208" s="8"/>
+      <c r="C208" s="9"/>
+      <c r="D208" s="8"/>
       <c r="E208" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="F208" s="10"/>
+      <c r="F208" s="9"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A209" s="9"/>
-      <c r="B209" s="9"/>
-      <c r="C209" s="10"/>
-      <c r="D209" s="9"/>
+      <c r="A209" s="8"/>
+      <c r="B209" s="8"/>
+      <c r="C209" s="9"/>
+      <c r="D209" s="8"/>
       <c r="E209" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="F209" s="10"/>
+      <c r="F209" s="9"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A210" s="8">
+      <c r="A210" s="6">
         <v>55</v>
       </c>
-      <c r="B210" s="8" t="s">
+      <c r="B210" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C210" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="D210" s="8" t="s">
+      <c r="D210" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E210" s="13" t="s">
+      <c r="E210" t="s">
         <v>213</v>
       </c>
-      <c r="F210" s="16" t="s">
+      <c r="F210" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A211" s="8"/>
-      <c r="B211" s="8"/>
+      <c r="A211" s="6"/>
+      <c r="B211" s="6"/>
       <c r="C211" s="7"/>
-      <c r="D211" s="8"/>
+      <c r="D211" s="6"/>
       <c r="E211" t="s">
         <v>214</v>
       </c>
-      <c r="F211" s="16"/>
+      <c r="F211" s="7"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A212" s="8"/>
-      <c r="B212" s="8"/>
+      <c r="A212" s="6"/>
+      <c r="B212" s="6"/>
       <c r="C212" s="7"/>
-      <c r="D212" s="8"/>
+      <c r="D212" s="6"/>
       <c r="E212" t="s">
         <v>215</v>
       </c>
-      <c r="F212" s="16"/>
+      <c r="F212" s="7"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" s="8"/>
-      <c r="B213" s="8"/>
+      <c r="A213" s="6"/>
+      <c r="B213" s="6"/>
       <c r="C213" s="7"/>
-      <c r="D213" s="8"/>
+      <c r="D213" s="6"/>
       <c r="E213" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F213" s="16"/>
+      <c r="F213" s="7"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A214" s="8"/>
-      <c r="B214" s="8"/>
+      <c r="A214" s="6"/>
+      <c r="B214" s="6"/>
       <c r="C214" s="7"/>
-      <c r="D214" s="8"/>
+      <c r="D214" s="6"/>
       <c r="E214" t="s">
-        <v>228</v>
-      </c>
-      <c r="F214" s="16"/>
+        <v>227</v>
+      </c>
+      <c r="F214" s="7"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A215" s="8"/>
-      <c r="B215" s="8"/>
+      <c r="A215" s="6"/>
+      <c r="B215" s="6"/>
       <c r="C215" s="7"/>
-      <c r="D215" s="8"/>
+      <c r="D215" s="6"/>
       <c r="E215" t="s">
         <v>163</v>
       </c>
-      <c r="F215" s="16"/>
+      <c r="F215" s="7"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A216" s="8">
+      <c r="A216" s="6">
         <v>56</v>
       </c>
-      <c r="B216" s="8" t="s">
+      <c r="B216" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="D216" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D216" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E216" s="13" t="s">
+      <c r="E216" t="s">
         <v>213</v>
       </c>
-      <c r="F216" s="16" t="s">
+      <c r="F216" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A217" s="8"/>
-      <c r="B217" s="8"/>
+      <c r="A217" s="6"/>
+      <c r="B217" s="6"/>
       <c r="C217" s="7"/>
-      <c r="D217" s="8"/>
+      <c r="D217" s="6"/>
       <c r="E217" t="s">
         <v>214</v>
       </c>
-      <c r="F217" s="16"/>
+      <c r="F217" s="7"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A218" s="8"/>
-      <c r="B218" s="8"/>
+      <c r="A218" s="6"/>
+      <c r="B218" s="6"/>
       <c r="C218" s="7"/>
-      <c r="D218" s="8"/>
+      <c r="D218" s="6"/>
       <c r="E218" t="s">
         <v>215</v>
       </c>
-      <c r="F218" s="16"/>
+      <c r="F218" s="7"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A219" s="8"/>
-      <c r="B219" s="8"/>
+      <c r="A219" s="6"/>
+      <c r="B219" s="6"/>
       <c r="C219" s="7"/>
-      <c r="D219" s="8"/>
+      <c r="D219" s="6"/>
       <c r="E219" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F219" s="16"/>
+      <c r="F219" s="7"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A220" s="8"/>
-      <c r="B220" s="8"/>
+      <c r="A220" s="6"/>
+      <c r="B220" s="6"/>
       <c r="C220" s="7"/>
-      <c r="D220" s="8"/>
+      <c r="D220" s="6"/>
       <c r="E220" t="s">
-        <v>229</v>
-      </c>
-      <c r="F220" s="16"/>
+        <v>228</v>
+      </c>
+      <c r="F220" s="7"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A221" s="8"/>
-      <c r="B221" s="8"/>
+      <c r="A221" s="6"/>
+      <c r="B221" s="6"/>
       <c r="C221" s="7"/>
-      <c r="D221" s="8"/>
+      <c r="D221" s="6"/>
       <c r="E221" t="s">
         <v>163</v>
       </c>
-      <c r="F221" s="16"/>
+      <c r="F221" s="7"/>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>226</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="300">
-    <mergeCell ref="D216:D221"/>
-    <mergeCell ref="F216:F221"/>
-    <mergeCell ref="C216:C221"/>
-    <mergeCell ref="B216:B221"/>
-    <mergeCell ref="A216:A221"/>
-    <mergeCell ref="A204:A209"/>
-    <mergeCell ref="B204:B209"/>
-    <mergeCell ref="C204:C209"/>
-    <mergeCell ref="D204:D209"/>
-    <mergeCell ref="F204:F209"/>
-    <mergeCell ref="A210:A215"/>
-    <mergeCell ref="B210:B215"/>
-    <mergeCell ref="C210:C215"/>
-    <mergeCell ref="D210:D215"/>
-    <mergeCell ref="F210:F215"/>
-    <mergeCell ref="F192:F197"/>
-    <mergeCell ref="D192:D197"/>
-    <mergeCell ref="C192:C197"/>
-    <mergeCell ref="B192:B197"/>
-    <mergeCell ref="A192:A197"/>
-    <mergeCell ref="A198:A203"/>
-    <mergeCell ref="B198:B203"/>
-    <mergeCell ref="C198:C203"/>
-    <mergeCell ref="D198:D203"/>
-    <mergeCell ref="F198:F203"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B189"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="F186:F187"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="F178:F179"/>
-    <mergeCell ref="D180:D181"/>
-    <mergeCell ref="F180:F181"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="B182:B185"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="F182:F183"/>
-    <mergeCell ref="D184:D185"/>
-    <mergeCell ref="F184:F185"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B174:B177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="D176:D177"/>
-    <mergeCell ref="F176:F177"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="F58:F60"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="D55:D57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="A167:A169"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="B162:B166"/>
+    <mergeCell ref="C162:C166"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="F162:F166"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="B157:B161"/>
+    <mergeCell ref="C157:C161"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="F157:F161"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="C152:C156"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="F152:F156"/>
+    <mergeCell ref="D154:D156"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="C147:C151"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="F147:F151"/>
+    <mergeCell ref="D149:D151"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="D144:D146"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="C137:C141"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="F137:F141"/>
+    <mergeCell ref="D139:D141"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="C132:C136"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="F132:F136"/>
+    <mergeCell ref="D134:D136"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="C127:C131"/>
+    <mergeCell ref="D127:D128"/>
+    <mergeCell ref="F127:F131"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="C122:C126"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="F122:F126"/>
+    <mergeCell ref="D124:D126"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="F117:F121"/>
+    <mergeCell ref="B112:B116"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="B117:B121"/>
+    <mergeCell ref="C117:C121"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="F114:F116"/>
+    <mergeCell ref="F112:F113"/>
+    <mergeCell ref="D114:D116"/>
+    <mergeCell ref="C112:C116"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="F96:F99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="D94:D95"/>
     <mergeCell ref="A88:A91"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="C88:C91"/>
@@ -4219,110 +4454,181 @@
     <mergeCell ref="D78:D79"/>
     <mergeCell ref="C76:C79"/>
     <mergeCell ref="B76:B79"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="F96:F99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="F92:F95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D102:D103"/>
-    <mergeCell ref="B112:B116"/>
-    <mergeCell ref="A112:A116"/>
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="B117:B121"/>
-    <mergeCell ref="C117:C121"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="F114:F116"/>
-    <mergeCell ref="F112:F113"/>
-    <mergeCell ref="D114:D116"/>
-    <mergeCell ref="C112:C116"/>
-    <mergeCell ref="A122:A126"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="C122:C126"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="F122:F126"/>
-    <mergeCell ref="D124:D126"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="F117:F121"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="C137:C141"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="F137:F141"/>
-    <mergeCell ref="D139:D141"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="C132:C136"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="F132:F136"/>
-    <mergeCell ref="D134:D136"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="C127:C131"/>
-    <mergeCell ref="D127:D128"/>
-    <mergeCell ref="F127:F131"/>
-    <mergeCell ref="D129:D131"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="C147:C151"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="F147:F151"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="F142:F146"/>
-    <mergeCell ref="D144:D146"/>
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="B157:B161"/>
-    <mergeCell ref="C157:C161"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="F157:F161"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="A152:A156"/>
-    <mergeCell ref="B152:B156"/>
-    <mergeCell ref="C152:C156"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="F152:F156"/>
-    <mergeCell ref="D154:D156"/>
-    <mergeCell ref="F167:F169"/>
-    <mergeCell ref="D168:D169"/>
-    <mergeCell ref="C167:C169"/>
-    <mergeCell ref="B167:B169"/>
-    <mergeCell ref="A167:A169"/>
-    <mergeCell ref="A162:A166"/>
-    <mergeCell ref="B162:B166"/>
-    <mergeCell ref="C162:C166"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="F162:F166"/>
-    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="F58:F60"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B174:B177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="D176:D177"/>
+    <mergeCell ref="F176:F177"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="F178:F179"/>
+    <mergeCell ref="D180:D181"/>
+    <mergeCell ref="F180:F181"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="B182:B185"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="F182:F183"/>
+    <mergeCell ref="D184:D185"/>
+    <mergeCell ref="F184:F185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B189"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="F186:F187"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="C190:C191"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="F192:F197"/>
+    <mergeCell ref="D192:D197"/>
+    <mergeCell ref="C192:C197"/>
+    <mergeCell ref="B192:B197"/>
+    <mergeCell ref="A192:A197"/>
+    <mergeCell ref="A198:A203"/>
+    <mergeCell ref="B198:B203"/>
+    <mergeCell ref="C198:C203"/>
+    <mergeCell ref="D198:D203"/>
+    <mergeCell ref="F198:F203"/>
+    <mergeCell ref="D216:D221"/>
+    <mergeCell ref="F216:F221"/>
+    <mergeCell ref="C216:C221"/>
+    <mergeCell ref="B216:B221"/>
+    <mergeCell ref="A216:A221"/>
+    <mergeCell ref="A204:A209"/>
+    <mergeCell ref="B204:B209"/>
+    <mergeCell ref="C204:C209"/>
+    <mergeCell ref="D204:D209"/>
+    <mergeCell ref="F204:F209"/>
+    <mergeCell ref="A210:A215"/>
+    <mergeCell ref="B210:B215"/>
+    <mergeCell ref="C210:C215"/>
+    <mergeCell ref="D210:D215"/>
+    <mergeCell ref="F210:F215"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>